<commit_message>
assignment 1 and class work
</commit_message>
<xml_diff>
--- a/DataFiles/CH 08/Bicycle.xlsx
+++ b/DataFiles/CH 08/Bicycle.xlsx
@@ -1,45 +1,149 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fryml.BUSINESS\Documents\My Dropbox\ASW Files\BusAnalytics (EBA)\FINAL CHAPTER FILES\05_Chapter5_Time Series Forecasting_JIM\bookDisk\WEBfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andyconverse/Documents/Hamline Acedmics/Hamline 2024-25/Hamline Spring 25/QMBE 3730/QMBE_3730_Andy_Converse/Untitled/DataFiles/CH 08/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D169CC9-7F40-1443-8E37-BADE52610731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="14865" windowHeight="8580"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Year</t>
   </si>
   <si>
     <t>Sales</t>
+  </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
+  <si>
+    <t>RESIDUAL OUTPUT</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>Predicted Sales</t>
+  </si>
+  <si>
+    <t>Residuals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -53,7 +157,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -61,14 +165,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -88,9 +220,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -128,9 +260,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -165,7 +297,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,7 +332,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -373,16 +505,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -390,15 +522,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>21.6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -406,55 +541,89 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>21.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.87452616661188121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>23.9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.76479601608887182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.73539551809998083</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>31.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.9589538024159734</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>29.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -462,12 +631,296 @@
         <v>28.6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>31.4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>99.825000000000003</v>
+      </c>
+      <c r="G13" s="2">
+        <v>99.825000000000003</v>
+      </c>
+      <c r="H13" s="2">
+        <v>26.013029315960907</v>
+      </c>
+      <c r="I13" s="2">
+        <v>9.2950922339240366E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2">
+        <v>8</v>
+      </c>
+      <c r="F14" s="2">
+        <v>30.700000000000006</v>
+      </c>
+      <c r="G14" s="2">
+        <v>3.8375000000000008</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="3">
+        <v>9</v>
+      </c>
+      <c r="F15" s="3">
+        <v>130.52500000000001</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="2">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1.3382202110763886</v>
+      </c>
+      <c r="G18" s="2">
+        <v>15.244127858143312</v>
+      </c>
+      <c r="H18" s="2">
+        <v>3.3998882786469612E-7</v>
+      </c>
+      <c r="I18" s="2">
+        <v>17.314058659444054</v>
+      </c>
+      <c r="J18" s="2">
+        <v>23.485941340555943</v>
+      </c>
+      <c r="K18" s="2">
+        <v>17.314058659444054</v>
+      </c>
+      <c r="L18" s="2">
+        <v>23.485941340555943</v>
+      </c>
+    </row>
+    <row r="19" spans="4:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1.1000000000000005</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.21567371540164909</v>
+      </c>
+      <c r="G19" s="3">
+        <v>5.1002969831139175</v>
+      </c>
+      <c r="H19" s="3">
+        <v>9.2950922339240117E-4</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0.6026555204289511</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1.5973444795710501</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0.6026555204289511</v>
+      </c>
+      <c r="L19" s="3">
+        <v>1.5973444795710501</v>
+      </c>
+    </row>
+    <row r="23" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="4:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2">
+        <v>21.5</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.10000000000000142</v>
+      </c>
+    </row>
+    <row r="27" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D27" s="2">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2">
+        <v>22.6</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.29999999999999716</v>
+      </c>
+    </row>
+    <row r="28" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D28" s="2">
+        <v>3</v>
+      </c>
+      <c r="E28" s="2">
+        <v>23.7</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1.8000000000000007</v>
+      </c>
+    </row>
+    <row r="29" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D29" s="2">
+        <v>4</v>
+      </c>
+      <c r="E29" s="2">
+        <v>24.8</v>
+      </c>
+      <c r="F29" s="2">
+        <v>-2.9000000000000021</v>
+      </c>
+    </row>
+    <row r="30" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D30" s="2">
+        <v>5</v>
+      </c>
+      <c r="E30" s="2">
+        <v>25.900000000000002</v>
+      </c>
+      <c r="F30" s="2">
+        <v>-2.0000000000000036</v>
+      </c>
+    </row>
+    <row r="31" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D31" s="2">
+        <v>6</v>
+      </c>
+      <c r="E31" s="2">
+        <v>27</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D32" s="2">
+        <v>7</v>
+      </c>
+      <c r="E32" s="2">
+        <v>28.1</v>
+      </c>
+      <c r="F32" s="2">
+        <v>3.3999999999999986</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D33" s="2">
+        <v>8</v>
+      </c>
+      <c r="E33" s="2">
+        <v>29.200000000000003</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.49999999999999645</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D34" s="2">
+        <v>9</v>
+      </c>
+      <c r="E34" s="2">
+        <v>30.300000000000004</v>
+      </c>
+      <c r="F34" s="2">
+        <v>-1.7000000000000028</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="3">
+        <v>10</v>
+      </c>
+      <c r="E35" s="3">
+        <v>31.400000000000006</v>
+      </c>
+      <c r="F35" s="3">
+        <v>-7.1054273576010019E-15</v>
       </c>
     </row>
   </sheetData>
@@ -478,12 +931,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -492,12 +945,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>